<commit_message>
add classification and update structure
</commit_message>
<xml_diff>
--- a/Pith2Bark/dataset/tracy.xlsx
+++ b/Pith2Bark/dataset/tracy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammadfarooq/Codebase/thesis-experiment/Pith2Bark/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BF24DC-95FA-CB4B-9705-A64A5DB5AE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C76297-9C58-AE4D-9D6F-4C149121949C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="3600" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -398,9 +398,11 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>114</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="C2" s="1">
+        <v>130</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -410,9 +412,11 @@
         <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>141</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="C3" s="1">
+        <v>109</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -422,9 +426,11 @@
         <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>248</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>244</v>
+      </c>
+      <c r="C4" s="1">
+        <v>222</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -436,7 +442,9 @@
       <c r="B5" s="1">
         <v>130</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>116</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
@@ -445,9 +453,11 @@
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>140</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="C6" s="1">
+        <v>113</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
@@ -456,9 +466,11 @@
         <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>161</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="C7" s="1">
+        <v>124</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
@@ -469,7 +481,9 @@
       <c r="B8" s="1">
         <v>129</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>118</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
@@ -480,7 +494,9 @@
       <c r="B9" s="1">
         <v>114</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>124</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -492,7 +508,9 @@
       <c r="B10" s="1">
         <v>90</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>80</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
@@ -501,9 +519,11 @@
         <v>15</v>
       </c>
       <c r="B11" s="1">
-        <v>89</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C11" s="1">
+        <v>68</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -511,7 +531,10 @@
         <v>16</v>
       </c>
       <c r="B12" s="1">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="C12" s="1">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -521,13 +544,19 @@
       <c r="B13" s="1">
         <v>90</v>
       </c>
+      <c r="C13" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="1">
-        <v>93</v>
+        <v>83</v>
+      </c>
+      <c r="C14" s="1">
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -537,6 +566,9 @@
       <c r="B15" s="1">
         <v>84</v>
       </c>
+      <c r="C15" s="1">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -545,61 +577,85 @@
       <c r="B16" s="1">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C16" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>89</v>
+      </c>
+      <c r="C17" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>88</v>
+      </c>
+      <c r="C18" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="1">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+      <c r="C19" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C20" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C22" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="1">
         <v>101</v>
+      </c>
+      <c r="C23" s="1">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>